<commit_message>
v0.1 improvement of meta-information about annotation run
</commit_message>
<xml_diff>
--- a/molgenis-data-annotators/src/test/resources/GeneNetworkAnnotator.xlsx
+++ b/molgenis-data-annotators/src/test/resources/GeneNetworkAnnotator.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>name</t>
   </si>
@@ -147,10 +147,22 @@
     <t>xref</t>
   </si>
   <si>
-    <t>Annotation_log</t>
-  </si>
-  <si>
-    <t>Annotation log</t>
+    <t>termsFound</t>
+  </si>
+  <si>
+    <t>termsNotFound</t>
+  </si>
+  <si>
+    <t>terms used for Gene Network</t>
+  </si>
+  <si>
+    <t>termsnot  used for Gene Network</t>
+  </si>
+  <si>
+    <t>HPO terms that were used by the gene network annotator</t>
+  </si>
+  <si>
+    <t>HPO terms that were not found by the gene network annotator</t>
   </si>
 </sst>
 </file>
@@ -240,10 +252,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -271,7 +291,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="25">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -280,6 +300,10 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -287,6 +311,10 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -617,17 +645,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" customWidth="1"/>
     <col min="4" max="4" width="65" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
     <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
@@ -744,7 +772,7 @@
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -758,13 +786,13 @@
       </c>
     </row>
     <row r="6" spans="1:15" s="3" customFormat="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -782,49 +810,70 @@
         <v>36</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:15" s="3" customFormat="1">
+      <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="2" customFormat="1">
-      <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="B8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="H8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:15" s="2" customFormat="1">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="2" customFormat="1">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
initial version of url file upload + fix for checking the importrun object
</commit_message>
<xml_diff>
--- a/molgenis-data-annotators/src/test/resources/GeneNetworkAnnotator.xlsx
+++ b/molgenis-data-annotators/src/test/resources/GeneNetworkAnnotator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="attributes" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>name</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t>HPO terms that were not found by the gene network annotator</t>
+  </si>
+  <si>
+    <t>geneNetworkLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gene Network URL</t>
+  </si>
+  <si>
+    <t>Link to the gene network page for the HPO terms for this project</t>
+  </si>
+  <si>
+    <t>hyperlink</t>
   </si>
 </sst>
 </file>
@@ -252,7 +264,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -278,8 +290,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
@@ -290,8 +304,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="27">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -304,6 +321,7 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -315,6 +333,7 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -645,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -837,43 +856,60 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="2" customFormat="1">
-      <c r="A9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2" t="b">
-        <v>1</v>
+    <row r="9" spans="1:15" s="3" customFormat="1">
+      <c r="A9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:15" s="2" customFormat="1">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="2" customFormat="1">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>